<commit_message>
add experiment times estimates + MOBILESoft metadata
</commit_message>
<xml_diff>
--- a/resources/top_apps/top5_apks_metadata/dm_123apps_210sec_run.xlsx
+++ b/resources/top_apps/top5_apks_metadata/dm_123apps_210sec_run.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -761,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update various (meta-)data + add legacy-results
</commit_message>
<xml_diff>
--- a/resources/top_apps/top5_apks_metadata/dm_123apps_210sec_run.xlsx
+++ b/resources/top_apps/top5_apks_metadata/dm_123apps_210sec_run.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="127">
   <si>
     <t>seconds</t>
   </si>
@@ -408,18 +408,6 @@
   </si>
   <si>
     <t>unique_event_apis</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -792,7 +780,7 @@
   <dimension ref="A1:F124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>